<commit_message>
Refactor forecasting functions and improve documentation for clarity
</commit_message>
<xml_diff>
--- a/data/accurate_my_wind_speed_and_solar_data.xlsx
+++ b/data/accurate_my_wind_speed_and_solar_data.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHRISTOPHER\Documents\MATLAB\MicrogridSim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A93F10-F4F4-48C8-A705-D8F1E71A2E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7583898-9D80-4E96-B52B-769E7CFD9667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="2880" windowWidth="12510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="3570" windowWidth="12510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -30,10 +28,10 @@
     <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> G</t>
+    <t>G</t>
   </si>
   <si>
-    <t xml:space="preserve"> W_S</t>
+    <t>W_S</t>
   </si>
 </sst>
 </file>
@@ -78,24 +76,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -404,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +670,10 @@
       <c r="B20" s="2">
         <v>0.79175925925925927</v>
       </c>
-      <c r="C20" s="17">
-        <v>0</v>
-      </c>
-      <c r="D20" s="17">
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -700,10 +684,10 @@
       <c r="B21" s="2">
         <v>0.8334259259259259</v>
       </c>
-      <c r="C21" s="17">
-        <v>0</v>
-      </c>
-      <c r="D21" s="17">
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -714,10 +698,10 @@
       <c r="B22" s="2">
         <v>0.87509259259259264</v>
       </c>
-      <c r="C22" s="17">
-        <v>0</v>
-      </c>
-      <c r="D22" s="17">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1022,10 +1006,10 @@
       <c r="B44" s="2">
         <v>0.79197916666666668</v>
       </c>
-      <c r="C44" s="16">
-        <v>0</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1036,10 +1020,10 @@
       <c r="B45" s="2">
         <v>0.83364583333333331</v>
       </c>
-      <c r="C45" s="16">
-        <v>0</v>
-      </c>
-      <c r="D45" s="16">
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1050,10 +1034,10 @@
       <c r="B46" s="2">
         <v>0.87531250000000005</v>
       </c>
-      <c r="C46" s="16">
-        <v>0</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1064,10 +1048,10 @@
       <c r="B47" s="2">
         <v>0.91697916666666668</v>
       </c>
-      <c r="C47" s="16">
-        <v>0</v>
-      </c>
-      <c r="D47" s="16">
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1078,10 +1062,10 @@
       <c r="B48" s="2">
         <v>0.95864583333333331</v>
       </c>
-      <c r="C48" s="16">
-        <v>0</v>
-      </c>
-      <c r="D48" s="16">
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1092,10 +1076,10 @@
       <c r="B49" s="2">
         <v>3.1250000000000001E-4</v>
       </c>
-      <c r="C49" s="16">
-        <v>0</v>
-      </c>
-      <c r="D49" s="16">
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1358,10 +1342,10 @@
       <c r="B68" s="2">
         <v>0.7920949074074074</v>
       </c>
-      <c r="C68" s="15">
-        <v>0</v>
-      </c>
-      <c r="D68" s="15">
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1372,10 +1356,10 @@
       <c r="B69" s="2">
         <v>0.83376157407407403</v>
       </c>
-      <c r="C69" s="15">
-        <v>0</v>
-      </c>
-      <c r="D69" s="15">
+      <c r="C69" s="3">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1386,10 +1370,10 @@
       <c r="B70" s="2">
         <v>0.87542824074074077</v>
       </c>
-      <c r="C70" s="15">
-        <v>0</v>
-      </c>
-      <c r="D70" s="15">
+      <c r="C70" s="3">
+        <v>0</v>
+      </c>
+      <c r="D70" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1400,10 +1384,10 @@
       <c r="B71" s="2">
         <v>0.9170949074074074</v>
       </c>
-      <c r="C71" s="15">
-        <v>0</v>
-      </c>
-      <c r="D71" s="15">
+      <c r="C71" s="3">
+        <v>0</v>
+      </c>
+      <c r="D71" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1414,10 +1398,10 @@
       <c r="B72" s="2">
         <v>0.95876157407407403</v>
       </c>
-      <c r="C72" s="15">
-        <v>0</v>
-      </c>
-      <c r="D72" s="15">
+      <c r="C72" s="3">
+        <v>0</v>
+      </c>
+      <c r="D72" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1428,10 +1412,10 @@
       <c r="B73" s="2">
         <v>4.2824074074074075E-4</v>
       </c>
-      <c r="C73" s="15">
-        <v>0</v>
-      </c>
-      <c r="D73" s="15">
+      <c r="C73" s="3">
+        <v>0</v>
+      </c>
+      <c r="D73" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1694,10 +1678,10 @@
       <c r="B92" s="2">
         <v>0.79182870370370373</v>
       </c>
-      <c r="C92" s="14">
-        <v>0</v>
-      </c>
-      <c r="D92" s="14">
+      <c r="C92" s="3">
+        <v>0</v>
+      </c>
+      <c r="D92" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1708,10 +1692,10 @@
       <c r="B93" s="2">
         <v>0.83349537037037036</v>
       </c>
-      <c r="C93" s="14">
-        <v>0</v>
-      </c>
-      <c r="D93" s="14">
+      <c r="C93" s="3">
+        <v>0</v>
+      </c>
+      <c r="D93" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1722,10 +1706,10 @@
       <c r="B94" s="2">
         <v>0.87516203703703699</v>
       </c>
-      <c r="C94" s="14">
-        <v>0</v>
-      </c>
-      <c r="D94" s="14">
+      <c r="C94" s="3">
+        <v>0</v>
+      </c>
+      <c r="D94" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1736,10 +1720,10 @@
       <c r="B95" s="2">
         <v>0.91682870370370373</v>
       </c>
-      <c r="C95" s="14">
-        <v>0</v>
-      </c>
-      <c r="D95" s="14">
+      <c r="C95" s="3">
+        <v>0</v>
+      </c>
+      <c r="D95" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1750,10 +1734,10 @@
       <c r="B96" s="2">
         <v>0.95849537037037036</v>
       </c>
-      <c r="C96" s="14">
-        <v>0</v>
-      </c>
-      <c r="D96" s="14">
+      <c r="C96" s="3">
+        <v>0</v>
+      </c>
+      <c r="D96" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -1764,10 +1748,10 @@
       <c r="B97" s="2">
         <v>1.6203703703703703E-4</v>
       </c>
-      <c r="C97" s="14">
-        <v>0</v>
-      </c>
-      <c r="D97" s="14">
+      <c r="C97" s="3">
+        <v>0</v>
+      </c>
+      <c r="D97" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2030,10 +2014,10 @@
       <c r="B116" s="2">
         <v>0.79184027777777777</v>
       </c>
-      <c r="C116" s="13">
-        <v>0</v>
-      </c>
-      <c r="D116" s="13">
+      <c r="C116" s="3">
+        <v>0</v>
+      </c>
+      <c r="D116" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2044,10 +2028,10 @@
       <c r="B117" s="2">
         <v>0.8335069444444444</v>
       </c>
-      <c r="C117" s="13">
-        <v>0</v>
-      </c>
-      <c r="D117" s="13">
+      <c r="C117" s="3">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2058,10 +2042,10 @@
       <c r="B118" s="2">
         <v>0.87517361111111114</v>
       </c>
-      <c r="C118" s="13">
-        <v>0</v>
-      </c>
-      <c r="D118" s="13">
+      <c r="C118" s="3">
+        <v>0</v>
+      </c>
+      <c r="D118" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2072,10 +2056,10 @@
       <c r="B119" s="2">
         <v>0.91684027777777777</v>
       </c>
-      <c r="C119" s="13">
-        <v>0</v>
-      </c>
-      <c r="D119" s="13">
+      <c r="C119" s="3">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2086,10 +2070,10 @@
       <c r="B120" s="2">
         <v>0.9585069444444444</v>
       </c>
-      <c r="C120" s="13">
-        <v>0</v>
-      </c>
-      <c r="D120" s="13">
+      <c r="C120" s="3">
+        <v>0</v>
+      </c>
+      <c r="D120" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2100,10 +2084,10 @@
       <c r="B121" s="2">
         <v>1.7361111111111112E-4</v>
       </c>
-      <c r="C121" s="13">
-        <v>0</v>
-      </c>
-      <c r="D121" s="13">
+      <c r="C121" s="3">
+        <v>0</v>
+      </c>
+      <c r="D121" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2366,10 +2350,10 @@
       <c r="B140" s="2">
         <v>0.79167824074074078</v>
       </c>
-      <c r="C140" s="12">
-        <v>0</v>
-      </c>
-      <c r="D140" s="12">
+      <c r="C140" s="3">
+        <v>0</v>
+      </c>
+      <c r="D140" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2380,10 +2364,10 @@
       <c r="B141" s="2">
         <v>0.83334490740740741</v>
       </c>
-      <c r="C141" s="12">
-        <v>0</v>
-      </c>
-      <c r="D141" s="12">
+      <c r="C141" s="3">
+        <v>0</v>
+      </c>
+      <c r="D141" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2394,10 +2378,10 @@
       <c r="B142" s="2">
         <v>0.87501157407407404</v>
       </c>
-      <c r="C142" s="12">
-        <v>0</v>
-      </c>
-      <c r="D142" s="12">
+      <c r="C142" s="3">
+        <v>0</v>
+      </c>
+      <c r="D142" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2408,10 +2392,10 @@
       <c r="B143" s="2">
         <v>0.91667824074074078</v>
       </c>
-      <c r="C143" s="12">
-        <v>0</v>
-      </c>
-      <c r="D143" s="12">
+      <c r="C143" s="3">
+        <v>0</v>
+      </c>
+      <c r="D143" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2422,10 +2406,10 @@
       <c r="B144" s="2">
         <v>0.95834490740740741</v>
       </c>
-      <c r="C144" s="12">
-        <v>0</v>
-      </c>
-      <c r="D144" s="12">
+      <c r="C144" s="3">
+        <v>0</v>
+      </c>
+      <c r="D144" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2436,10 +2420,10 @@
       <c r="B145" s="2">
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="C145" s="12">
-        <v>0</v>
-      </c>
-      <c r="D145" s="12">
+      <c r="C145" s="3">
+        <v>0</v>
+      </c>
+      <c r="D145" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2702,10 +2686,10 @@
       <c r="B164" s="2">
         <v>0.79200231481481487</v>
       </c>
-      <c r="C164" s="11">
-        <v>0</v>
-      </c>
-      <c r="D164" s="11">
+      <c r="C164" s="3">
+        <v>0</v>
+      </c>
+      <c r="D164" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2716,10 +2700,10 @@
       <c r="B165" s="2">
         <v>0.8336689814814815</v>
       </c>
-      <c r="C165" s="11">
-        <v>0</v>
-      </c>
-      <c r="D165" s="11">
+      <c r="C165" s="3">
+        <v>0</v>
+      </c>
+      <c r="D165" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2730,10 +2714,10 @@
       <c r="B166" s="2">
         <v>0.87533564814814813</v>
       </c>
-      <c r="C166" s="11">
-        <v>0</v>
-      </c>
-      <c r="D166" s="11">
+      <c r="C166" s="3">
+        <v>0</v>
+      </c>
+      <c r="D166" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2744,10 +2728,10 @@
       <c r="B167" s="2">
         <v>0.91700231481481487</v>
       </c>
-      <c r="C167" s="11">
-        <v>0</v>
-      </c>
-      <c r="D167" s="11">
+      <c r="C167" s="3">
+        <v>0</v>
+      </c>
+      <c r="D167" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2758,10 +2742,10 @@
       <c r="B168" s="2">
         <v>0.9586689814814815</v>
       </c>
-      <c r="C168" s="11">
-        <v>0</v>
-      </c>
-      <c r="D168" s="11">
+      <c r="C168" s="3">
+        <v>0</v>
+      </c>
+      <c r="D168" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -2772,10 +2756,10 @@
       <c r="B169" s="2">
         <v>3.3564814814814812E-4</v>
       </c>
-      <c r="C169" s="11">
-        <v>0</v>
-      </c>
-      <c r="D169" s="11">
+      <c r="C169" s="3">
+        <v>0</v>
+      </c>
+      <c r="D169" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3038,10 +3022,10 @@
       <c r="B188" s="2">
         <v>0.79207175925925921</v>
       </c>
-      <c r="C188" s="10">
-        <v>0</v>
-      </c>
-      <c r="D188" s="10">
+      <c r="C188" s="3">
+        <v>0</v>
+      </c>
+      <c r="D188" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3052,10 +3036,10 @@
       <c r="B189" s="2">
         <v>0.83373842592592595</v>
       </c>
-      <c r="C189" s="10">
-        <v>0</v>
-      </c>
-      <c r="D189" s="10">
+      <c r="C189" s="3">
+        <v>0</v>
+      </c>
+      <c r="D189" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3066,10 +3050,10 @@
       <c r="B190" s="2">
         <v>0.87540509259259258</v>
       </c>
-      <c r="C190" s="10">
-        <v>0</v>
-      </c>
-      <c r="D190" s="10">
+      <c r="C190" s="3">
+        <v>0</v>
+      </c>
+      <c r="D190" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3080,10 +3064,10 @@
       <c r="B191" s="2">
         <v>0.91707175925925921</v>
       </c>
-      <c r="C191" s="10">
-        <v>0</v>
-      </c>
-      <c r="D191" s="10">
+      <c r="C191" s="3">
+        <v>0</v>
+      </c>
+      <c r="D191" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3094,10 +3078,10 @@
       <c r="B192" s="2">
         <v>0.95873842592592595</v>
       </c>
-      <c r="C192" s="10">
-        <v>0</v>
-      </c>
-      <c r="D192" s="10">
+      <c r="C192" s="3">
+        <v>0</v>
+      </c>
+      <c r="D192" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3108,10 +3092,10 @@
       <c r="B193" s="2">
         <v>4.0509259259259258E-4</v>
       </c>
-      <c r="C193" s="10">
-        <v>0</v>
-      </c>
-      <c r="D193" s="10">
+      <c r="C193" s="3">
+        <v>0</v>
+      </c>
+      <c r="D193" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3374,10 +3358,10 @@
       <c r="B212" s="2">
         <v>0.79211805555555559</v>
       </c>
-      <c r="C212" s="9">
-        <v>0</v>
-      </c>
-      <c r="D212" s="9">
+      <c r="C212" s="3">
+        <v>0</v>
+      </c>
+      <c r="D212" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3388,10 +3372,10 @@
       <c r="B213" s="2">
         <v>0.83378472222222222</v>
       </c>
-      <c r="C213" s="9">
-        <v>0</v>
-      </c>
-      <c r="D213" s="9">
+      <c r="C213" s="3">
+        <v>0</v>
+      </c>
+      <c r="D213" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3402,10 +3386,10 @@
       <c r="B214" s="2">
         <v>0.87545138888888885</v>
       </c>
-      <c r="C214" s="9">
-        <v>0</v>
-      </c>
-      <c r="D214" s="9">
+      <c r="C214" s="3">
+        <v>0</v>
+      </c>
+      <c r="D214" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3416,10 +3400,10 @@
       <c r="B215" s="2">
         <v>0.91711805555555559</v>
       </c>
-      <c r="C215" s="9">
-        <v>0</v>
-      </c>
-      <c r="D215" s="9">
+      <c r="C215" s="3">
+        <v>0</v>
+      </c>
+      <c r="D215" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3430,10 +3414,10 @@
       <c r="B216" s="2">
         <v>0.95878472222222222</v>
       </c>
-      <c r="C216" s="9">
-        <v>0</v>
-      </c>
-      <c r="D216" s="9">
+      <c r="C216" s="3">
+        <v>0</v>
+      </c>
+      <c r="D216" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3444,10 +3428,10 @@
       <c r="B217" s="2">
         <v>4.5138888888888887E-4</v>
       </c>
-      <c r="C217" s="9">
-        <v>0</v>
-      </c>
-      <c r="D217" s="9">
+      <c r="C217" s="3">
+        <v>0</v>
+      </c>
+      <c r="D217" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3710,10 +3694,10 @@
       <c r="B236" s="2">
         <v>0.79232638888888884</v>
       </c>
-      <c r="C236" s="8">
-        <v>0</v>
-      </c>
-      <c r="D236" s="8">
+      <c r="C236" s="3">
+        <v>0</v>
+      </c>
+      <c r="D236" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3724,10 +3708,10 @@
       <c r="B237" s="2">
         <v>0.83399305555555558</v>
       </c>
-      <c r="C237" s="8">
-        <v>0</v>
-      </c>
-      <c r="D237" s="8">
+      <c r="C237" s="3">
+        <v>0</v>
+      </c>
+      <c r="D237" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3738,10 +3722,10 @@
       <c r="B238" s="2">
         <v>0.87565972222222221</v>
       </c>
-      <c r="C238" s="8">
-        <v>0</v>
-      </c>
-      <c r="D238" s="8">
+      <c r="C238" s="3">
+        <v>0</v>
+      </c>
+      <c r="D238" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3752,10 +3736,10 @@
       <c r="B239" s="2">
         <v>0.91732638888888884</v>
       </c>
-      <c r="C239" s="8">
-        <v>0</v>
-      </c>
-      <c r="D239" s="8">
+      <c r="C239" s="3">
+        <v>0</v>
+      </c>
+      <c r="D239" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3766,10 +3750,10 @@
       <c r="B240" s="2">
         <v>0.95899305555555558</v>
       </c>
-      <c r="C240" s="8">
-        <v>0</v>
-      </c>
-      <c r="D240" s="8">
+      <c r="C240" s="3">
+        <v>0</v>
+      </c>
+      <c r="D240" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -3780,10 +3764,10 @@
       <c r="B241" s="2">
         <v>6.5972222222222224E-4</v>
       </c>
-      <c r="C241" s="8">
-        <v>0</v>
-      </c>
-      <c r="D241" s="8">
+      <c r="C241" s="3">
+        <v>0</v>
+      </c>
+      <c r="D241" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4046,10 +4030,10 @@
       <c r="B260" s="2">
         <v>0.7922569444444445</v>
       </c>
-      <c r="C260" s="7">
-        <v>0</v>
-      </c>
-      <c r="D260" s="7">
+      <c r="C260" s="3">
+        <v>0</v>
+      </c>
+      <c r="D260" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4060,10 +4044,10 @@
       <c r="B261" s="2">
         <v>0.83392361111111113</v>
       </c>
-      <c r="C261" s="7">
-        <v>0</v>
-      </c>
-      <c r="D261" s="7">
+      <c r="C261" s="3">
+        <v>0</v>
+      </c>
+      <c r="D261" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4074,10 +4058,10 @@
       <c r="B262" s="2">
         <v>0.87559027777777776</v>
       </c>
-      <c r="C262" s="7">
-        <v>0</v>
-      </c>
-      <c r="D262" s="7">
+      <c r="C262" s="3">
+        <v>0</v>
+      </c>
+      <c r="D262" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4088,10 +4072,10 @@
       <c r="B263" s="2">
         <v>0.9172569444444445</v>
       </c>
-      <c r="C263" s="7">
-        <v>0</v>
-      </c>
-      <c r="D263" s="7">
+      <c r="C263" s="3">
+        <v>0</v>
+      </c>
+      <c r="D263" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4102,10 +4086,10 @@
       <c r="B264" s="2">
         <v>0.95892361111111113</v>
       </c>
-      <c r="C264" s="7">
-        <v>0</v>
-      </c>
-      <c r="D264" s="7">
+      <c r="C264" s="3">
+        <v>0</v>
+      </c>
+      <c r="D264" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4116,10 +4100,10 @@
       <c r="B265" s="2">
         <v>5.9027777777777778E-4</v>
       </c>
-      <c r="C265" s="7">
-        <v>0</v>
-      </c>
-      <c r="D265" s="7">
+      <c r="C265" s="3">
+        <v>0</v>
+      </c>
+      <c r="D265" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4382,10 +4366,10 @@
       <c r="B284" s="2">
         <v>0.79204861111111113</v>
       </c>
-      <c r="C284" s="6">
-        <v>0</v>
-      </c>
-      <c r="D284" s="6">
+      <c r="C284" s="3">
+        <v>0</v>
+      </c>
+      <c r="D284" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4396,10 +4380,10 @@
       <c r="B285" s="2">
         <v>0.83371527777777776</v>
       </c>
-      <c r="C285" s="6">
-        <v>0</v>
-      </c>
-      <c r="D285" s="6">
+      <c r="C285" s="3">
+        <v>0</v>
+      </c>
+      <c r="D285" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4410,10 +4394,10 @@
       <c r="B286" s="2">
         <v>0.87538194444444439</v>
       </c>
-      <c r="C286" s="6">
-        <v>0</v>
-      </c>
-      <c r="D286" s="6">
+      <c r="C286" s="3">
+        <v>0</v>
+      </c>
+      <c r="D286" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4424,10 +4408,10 @@
       <c r="B287" s="2">
         <v>0.91704861111111113</v>
       </c>
-      <c r="C287" s="6">
-        <v>0</v>
-      </c>
-      <c r="D287" s="6">
+      <c r="C287" s="3">
+        <v>0</v>
+      </c>
+      <c r="D287" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4438,10 +4422,10 @@
       <c r="B288" s="2">
         <v>0.95871527777777776</v>
       </c>
-      <c r="C288" s="6">
-        <v>0</v>
-      </c>
-      <c r="D288" s="6">
+      <c r="C288" s="3">
+        <v>0</v>
+      </c>
+      <c r="D288" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4452,10 +4436,10 @@
       <c r="B289" s="2">
         <v>3.8194444444444446E-4</v>
       </c>
-      <c r="C289" s="6">
-        <v>0</v>
-      </c>
-      <c r="D289" s="6">
+      <c r="C289" s="3">
+        <v>0</v>
+      </c>
+      <c r="D289" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4718,10 +4702,10 @@
       <c r="B308" s="2">
         <v>0.79233796296296299</v>
       </c>
-      <c r="C308" s="4">
-        <v>0</v>
-      </c>
-      <c r="D308" s="4">
+      <c r="C308" s="3">
+        <v>0</v>
+      </c>
+      <c r="D308" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4732,10 +4716,10 @@
       <c r="B309" s="2">
         <v>0.83400462962962962</v>
       </c>
-      <c r="C309" s="4">
-        <v>0</v>
-      </c>
-      <c r="D309" s="4">
+      <c r="C309" s="3">
+        <v>0</v>
+      </c>
+      <c r="D309" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4746,10 +4730,10 @@
       <c r="B310" s="2">
         <v>0.87567129629629625</v>
       </c>
-      <c r="C310" s="4">
-        <v>0</v>
-      </c>
-      <c r="D310" s="4">
+      <c r="C310" s="3">
+        <v>0</v>
+      </c>
+      <c r="D310" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4760,10 +4744,10 @@
       <c r="B311" s="2">
         <v>0.91733796296296299</v>
       </c>
-      <c r="C311" s="4">
-        <v>0</v>
-      </c>
-      <c r="D311" s="4">
+      <c r="C311" s="3">
+        <v>0</v>
+      </c>
+      <c r="D311" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -4788,10 +4772,10 @@
       <c r="B313" s="2">
         <v>6.7129629629629625E-4</v>
       </c>
-      <c r="C313" s="5">
-        <v>0</v>
-      </c>
-      <c r="D313" s="5">
+      <c r="C313" s="3">
+        <v>0</v>
+      </c>
+      <c r="D313" s="3">
         <v>4.1455859374999999</v>
       </c>
     </row>
@@ -5135,28 +5119,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>